<commit_message>
Modify search_flights_input_data.xlsx and read_xlsx.py
</commit_message>
<xml_diff>
--- a/utils/search_flights_input_data.xlsx
+++ b/utils/search_flights_input_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\PROGRAMOWANIE\Software_Testing\Projects\phptravels-selenium-py\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339759A9-0E31-47CA-A6B1-B3972BFDBC5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA7F9D39-4783-4534-A84F-5EC1FAF7BDB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6150" yWindow="255" windowWidth="13350" windowHeight="15345" xr2:uid="{C9130730-17C0-4222-8D37-9CA77176A8F0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C9130730-17C0-4222-8D37-9CA77176A8F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
   <si>
     <t>cabin_class</t>
   </si>
@@ -125,7 +125,13 @@
     <t>JFK</t>
   </si>
   <si>
-    <t>current_year</t>
+    <t>trip_type</t>
+  </si>
+  <si>
+    <t>One Way</t>
+  </si>
+  <si>
+    <t>Round Trip</t>
   </si>
 </sst>
 </file>
@@ -481,15 +487,15 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
@@ -502,13 +508,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>30</v>
       </c>
       <c r="E1" t="s">
         <v>5</v>
@@ -543,13 +549,13 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>16</v>
-      </c>
-      <c r="D2">
-        <v>2019</v>
       </c>
       <c r="E2">
         <v>2019</v>
@@ -584,13 +590,13 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
         <v>17</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>18</v>
-      </c>
-      <c r="D3">
-        <v>2019</v>
       </c>
       <c r="E3">
         <v>2020</v>
@@ -625,13 +631,13 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
         <v>19</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>20</v>
-      </c>
-      <c r="D4">
-        <v>2019</v>
       </c>
       <c r="E4">
         <v>2019</v>
@@ -666,13 +672,13 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>22</v>
-      </c>
-      <c r="D5">
-        <v>2019</v>
       </c>
       <c r="E5">
         <v>2020</v>
@@ -707,13 +713,13 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
         <v>23</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>24</v>
-      </c>
-      <c r="D6">
-        <v>2019</v>
       </c>
       <c r="E6">
         <v>2019</v>
@@ -748,13 +754,13 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" t="s">
         <v>25</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>29</v>
-      </c>
-      <c r="D7">
-        <v>2019</v>
       </c>
       <c r="E7">
         <v>2019</v>

</xml_diff>

<commit_message>
Restore functions of setting trip type, modify test_search_flight
</commit_message>
<xml_diff>
--- a/utils/search_flights_input_data.xlsx
+++ b/utils/search_flights_input_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\PROGRAMOWANIE\Software_Testing\Projects\phptravels-selenium-py\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA7F9D39-4783-4534-A84F-5EC1FAF7BDB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F8C2F5-FA16-43C4-BA7A-2E354F63449C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C9130730-17C0-4222-8D37-9CA77176A8F0}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
   <si>
     <t>cabin_class</t>
   </si>
@@ -487,7 +487,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,12 +569,6 @@
       <c r="H2">
         <v>2019</v>
       </c>
-      <c r="I2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J2">
-        <v>17</v>
-      </c>
       <c r="K2">
         <v>2</v>
       </c>
@@ -610,12 +604,6 @@
       <c r="H3">
         <v>2020</v>
       </c>
-      <c r="I3" t="s">
-        <v>27</v>
-      </c>
-      <c r="J3">
-        <v>15</v>
-      </c>
       <c r="K3">
         <v>1</v>
       </c>
@@ -650,12 +638,6 @@
       </c>
       <c r="H4">
         <v>2019</v>
-      </c>
-      <c r="I4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J4">
-        <v>21</v>
       </c>
       <c r="K4">
         <v>0</v>

</xml_diff>

<commit_message>
Fix XlsxReder methods, modify tests
</commit_message>
<xml_diff>
--- a/utils/search_flights_input_data.xlsx
+++ b/utils/search_flights_input_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\PROGRAMOWANIE\Software_Testing\Projects\phptravels-selenium-py\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F8C2F5-FA16-43C4-BA7A-2E354F63449C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{447EFDFD-A560-43F8-9B4E-F7DD53F61FDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C9130730-17C0-4222-8D37-9CA77176A8F0}"/>
+    <workbookView xWindow="6150" yWindow="255" windowWidth="13350" windowHeight="15345" xr2:uid="{C9130730-17C0-4222-8D37-9CA77176A8F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
   <si>
     <t>cabin_class</t>
   </si>
@@ -123,15 +123,6 @@
   </si>
   <si>
     <t>JFK</t>
-  </si>
-  <si>
-    <t>trip_type</t>
-  </si>
-  <si>
-    <t>One Way</t>
-  </si>
-  <si>
-    <t>Round Trip</t>
   </si>
 </sst>
 </file>
@@ -484,291 +475,287 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64ED2AE4-BF9B-4B09-973D-AEE637327BED}">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" t="s">
         <v>16</v>
       </c>
-      <c r="E2">
+      <c r="D2">
         <v>2019</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E2" t="s">
         <v>26</v>
       </c>
+      <c r="F2">
+        <v>12</v>
+      </c>
       <c r="G2">
-        <v>12</v>
-      </c>
-      <c r="H2">
-        <v>2019</v>
+        <v>2020</v>
+      </c>
+      <c r="H2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2">
+        <v>6</v>
+      </c>
+      <c r="J2">
+        <v>2</v>
       </c>
       <c r="K2">
         <v>2</v>
       </c>
       <c r="L2">
-        <v>2</v>
-      </c>
-      <c r="M2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s">
         <v>18</v>
       </c>
-      <c r="E3">
+      <c r="D3">
         <v>2020</v>
       </c>
-      <c r="F3" t="s">
+      <c r="E3" t="s">
         <v>27</v>
       </c>
+      <c r="F3">
+        <v>9</v>
+      </c>
       <c r="G3">
-        <v>9</v>
-      </c>
-      <c r="H3">
         <v>2020</v>
       </c>
+      <c r="H3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3">
+        <v>6</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
       <c r="K3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L3">
         <v>0</v>
       </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
         <v>20</v>
       </c>
-      <c r="E4">
+      <c r="D4">
         <v>2019</v>
       </c>
-      <c r="F4" t="s">
+      <c r="E4" t="s">
         <v>26</v>
       </c>
+      <c r="F4">
+        <v>15</v>
+      </c>
       <c r="G4">
-        <v>15</v>
-      </c>
-      <c r="H4">
         <v>2019</v>
+      </c>
+      <c r="H4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4">
+        <v>14</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
       </c>
       <c r="K4">
         <v>0</v>
       </c>
       <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" t="s">
         <v>22</v>
       </c>
-      <c r="E5">
+      <c r="D5">
         <v>2020</v>
       </c>
-      <c r="F5" t="s">
+      <c r="E5" t="s">
         <v>28</v>
       </c>
+      <c r="F5">
+        <v>10</v>
+      </c>
       <c r="G5">
-        <v>10</v>
-      </c>
-      <c r="H5">
         <v>2020</v>
       </c>
-      <c r="I5" t="s">
+      <c r="H5" t="s">
         <v>28</v>
       </c>
+      <c r="I5">
+        <v>16</v>
+      </c>
       <c r="J5">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="K5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L5">
-        <v>1</v>
-      </c>
-      <c r="M5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" t="s">
         <v>24</v>
       </c>
-      <c r="E6">
+      <c r="D6">
         <v>2019</v>
       </c>
-      <c r="F6" t="s">
+      <c r="E6" t="s">
         <v>26</v>
       </c>
+      <c r="F6">
+        <v>31</v>
+      </c>
       <c r="G6">
-        <v>31</v>
-      </c>
-      <c r="H6">
         <v>2020</v>
       </c>
-      <c r="I6" t="s">
+      <c r="H6" t="s">
         <v>27</v>
       </c>
+      <c r="I6">
+        <v>6</v>
+      </c>
       <c r="J6">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="K6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L6">
-        <v>3</v>
-      </c>
-      <c r="M6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7">
+        <v>2019</v>
+      </c>
+      <c r="E7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7">
         <v>25</v>
       </c>
-      <c r="D7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7">
-        <v>2019</v>
-      </c>
-      <c r="F7" t="s">
-        <v>26</v>
-      </c>
       <c r="G7">
-        <v>25</v>
-      </c>
-      <c r="H7">
         <v>2020</v>
       </c>
-      <c r="I7" t="s">
+      <c r="H7" t="s">
         <v>27</v>
       </c>
+      <c r="I7">
+        <v>14</v>
+      </c>
       <c r="J7">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="K7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L7">
-        <v>2</v>
-      </c>
-      <c r="M7">
         <v>0</v>
       </c>
     </row>

</xml_diff>